<commit_message>
Fix debriefing end time in sample planning
</commit_message>
<xml_diff>
--- a/samples/example-planning.xlsx
+++ b/samples/example-planning.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\agenda-generator\samples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_clones\agenda-generator\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{EEC4942E-0886-49AA-8E51-C0EF3D003EED}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9450" yWindow="3240" windowWidth="12330" windowHeight="6060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9450" yWindow="3240" windowWidth="12330" windowHeight="6060"/>
   </bookViews>
   <sheets>
     <sheet name="Planning" sheetId="6" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="62">
   <si>
     <t>RECRUITMENT DAY XXX/XXX - XX/XX/2018</t>
   </si>
@@ -205,9 +204,6 @@
   </si>
   <si>
     <t>17:00 - 18:00</t>
-  </si>
-  <si>
-    <t>17:00 - 19:00</t>
   </si>
   <si>
     <t>DEBRIEFING (BE1749-Paris)</t>
@@ -219,7 +215,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="h:mm;@"/>
   </numFmts>
@@ -840,23 +836,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -892,23 +871,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1084,14 +1046,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A2:M46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1292,7 +1254,7 @@
         <v>59</v>
       </c>
       <c r="B15" s="37" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C15" s="38"/>
       <c r="D15" s="38"/>
@@ -1453,7 +1415,7 @@
         <v>59</v>
       </c>
       <c r="B28" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C28" s="9"/>
       <c r="D28" s="9"/>
@@ -1477,7 +1439,7 @@
         <v>2</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C31" s="9"/>
       <c r="D31" s="4" t="s">
@@ -1555,10 +1517,10 @@
     </row>
     <row r="39" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A39" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B39" s="25" t="s">
         <v>60</v>
-      </c>
-      <c r="B39" s="25" t="s">
-        <v>61</v>
       </c>
       <c r="C39" s="9"/>
       <c r="D39" s="9"/>
@@ -1592,7 +1554,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -1759,7 +1721,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0D58D4F-ADF0-4A64-8AB6-7857E1A33B11}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1816,5 +1778,8 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;R&amp;"Calibri"&amp;12 CONFIDENTIAL &amp; RESTRICTED&amp;1#</oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>